<commit_message>
fix stock card xls
</commit_message>
<xml_diff>
--- a/netforce_stock/netforce_stock/reports/stock_card.xlsx
+++ b/netforce_stock/netforce_stock/reports/stock_card.xlsx
@@ -97,7 +97,7 @@
     <t>{{currency in_qty}}</t>
   </si>
   <si>
-    <t>{{currency in_unit_price}}</t>
+    <t>{{currency in_cost_price}}</t>
   </si>
   <si>
     <t>{{currency in_amount}}</t>
@@ -109,7 +109,7 @@
     <t>{{currency out_qty}}</t>
   </si>
   <si>
-    <t>{{currency out_unit_price}}</t>
+    <t>{{currency out_cost_price}}</t>
   </si>
   <si>
     <t>{{currency out_amount}}</t>
@@ -471,12 +471,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -838,6 +839,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -864,6 +866,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
import report stock card
</commit_message>
<xml_diff>
--- a/netforce_stock/netforce_stock/reports/stock_card.xlsx
+++ b/netforce_stock/netforce_stock/reports/stock_card.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,151 +13,156 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
-    <t>Stock Card</t>
-  </si>
-  <si>
-    <t>{{company_name}}</t>
-  </si>
-  <si>
-    <t>Tax No {{tax_no}}</t>
-  </si>
-  <si>
-    <t>{{address}}</t>
-  </si>
-  <si>
-    <t>From {{date_from}} to {{date_to}}</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Ref</t>
-  </si>
-  <si>
-    <t>Lot / Serial Number</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>In</t>
-  </si>
-  <si>
-    <t>Out</t>
-  </si>
-  <si>
-    <t>Balance</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Unit Price</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Secondary Qty</t>
-  </si>
-  <si>
-    <t>Cost Price</t>
-  </si>
-  <si>
-    <t>Cost Amount</t>
-  </si>
-  <si>
-    <t>{{#each groups}}</t>
-  </si>
-  <si>
-    <t>{{product_name}} @ {{location_name}}</t>
-  </si>
-  <si>
-    <t>{{#each lines}}</t>
-  </si>
-  <si>
-    <t>{{date}}</t>
-  </si>
-  <si>
-    <t>{{ref}}</t>
-  </si>
-  <si>
-    <t>{{lot_num}}</t>
-  </si>
-  <si>
-    <t>{{invoice_num}}</t>
-  </si>
-  <si>
-    <t>{{currency in_qty}}</t>
-  </si>
-  <si>
-    <t>{{currency in_cost_price}}</t>
-  </si>
-  <si>
-    <t>{{currency in_amount}}</t>
-  </si>
-  <si>
-    <t>{{currency in_qty2}}</t>
-  </si>
-  <si>
-    <t>{{currency out_qty}}</t>
-  </si>
-  <si>
-    <t>{{currency out_cost_price}}</t>
-  </si>
-  <si>
-    <t>{{currency out_amount}}</t>
-  </si>
-  <si>
-    <t>{{currency out_qty2}}</t>
-  </si>
-  <si>
-    <t>{{currency bal_qty}}</t>
-  </si>
-  <si>
-    <t>{{currency bal_cost_price}}</t>
-  </si>
-  <si>
-    <t>{{currency bal_cost_amount}}</t>
-  </si>
-  <si>
-    <t>{{currency bal_qty2}}</t>
-  </si>
-  <si>
-    <t>{{#each landed_costs}}</t>
-  </si>
-  <si>
-    <t>{{currency amount}}</t>
-  </si>
-  <si>
-    <t>{{/each}}</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>{{currency total_in_qty}}</t>
-  </si>
-  <si>
-    <t>{{currency total_in_amount}}</t>
-  </si>
-  <si>
-    <t>{{currency total_in_qty2}}</t>
-  </si>
-  <si>
-    <t>{{currency total_out_qty}}</t>
-  </si>
-  <si>
-    <t>{{currency total_out_amount}}</t>
-  </si>
-  <si>
-    <t>{{currency total_out_qty2}}</t>
+    <t xml:space="preserve">Stock Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{company_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax No {{tax_no}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{address}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From {{date_from}} to {{date_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lot / Serial Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each groups}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{{product_code}}] {{product_name}} @ {{location_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each lines}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{date}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ref}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{lot_num}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{invoice_num}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency in_qty}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency in_cost_price}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency in_amount}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency in_qty2}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency out_qty}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency out_cost_price}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency out_amount}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency out_qty2}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency bal_qty}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency bal_cost_price}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency bal_cost_amount}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency bal_qty2}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each landed_costs}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency amount}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{/each}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_in_qty}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_in_amount}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_in_qty2}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_out_qty}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_out_amount}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_out_qty2}}</t>
   </si>
 </sst>
 </file>
@@ -165,7 +170,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -219,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -237,13 +242,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right style="hair"/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
       <top style="hair"/>
       <bottom/>
       <diagonal/>
@@ -323,7 +321,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -352,27 +350,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -380,15 +374,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -471,28 +465,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="20.0255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9948979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.0255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2908163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.015306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="17.484693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.9540816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.4948979591837"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.95408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -629,182 +623,182 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="12"/>
+      <c r="P11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="M12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="13" t="s">
+      <c r="N12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="O12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="13" t="s">
+      <c r="P12" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="12"/>
-    </row>
-    <row r="17" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15" t="s">
+      <c r="P16" s="11"/>
+    </row>
+    <row r="17" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15" t="s">
+      <c r="F17" s="14"/>
+      <c r="G17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15" t="s">
+      <c r="J17" s="14"/>
+      <c r="K17" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="16"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -812,7 +806,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F3:J3"/>
@@ -825,6 +819,7 @@
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="I6:L6"/>
     <mergeCell ref="M6:P6"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -839,7 +834,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -850,7 +845,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.95408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -866,7 +861,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -877,7 +872,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.95408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>